<commit_message>
finished touching up the reports tool in pandas
</commit_message>
<xml_diff>
--- a/HPM/2022/Reportes Py/01/Reporte_dropduplicates.xlsx
+++ b/HPM/2022/Reportes Py/01/Reporte_dropduplicates.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\All Projects\Python Projects\HPM\2022\Reportes Py\01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A67155-C665-437A-A148-BA0B94AAAD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -238,11 +232,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,14 +300,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -360,7 +346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,27 +378,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,24 +412,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -637,38 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,7 +662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>72710</v>
       </c>
@@ -792,7 +718,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>15514</v>
       </c>
@@ -848,7 +774,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>15527</v>
       </c>
@@ -904,7 +830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>65941</v>
       </c>
@@ -960,7 +886,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>79431</v>
       </c>
@@ -1016,7 +942,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>61275</v>
       </c>
@@ -1069,7 +995,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>14303</v>
       </c>
@@ -1122,7 +1048,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>42235</v>
       </c>
@@ -1178,7 +1104,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>41659</v>
       </c>
@@ -1231,7 +1157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>106416</v>
       </c>
@@ -1287,7 +1213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>23013</v>
       </c>
@@ -1343,7 +1269,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>83179</v>
       </c>
@@ -1399,7 +1325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>49033</v>
       </c>
@@ -1455,7 +1381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>32607</v>
       </c>
@@ -1511,7 +1437,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>61184</v>
       </c>

</xml_diff>